<commit_message>
MDT WIP procID -> ProcIdent
</commit_message>
<xml_diff>
--- a/MDT/DienstenCatalogus/BevoegdhedenEenT.xlsx
+++ b/MDT/DienstenCatalogus/BevoegdhedenEenT.xlsx
@@ -531,13 +531,13 @@
     <t>Systeem</t>
   </si>
   <si>
-    <t>ProcID</t>
-  </si>
-  <si>
     <t>BevoegdheidOmschrijving</t>
   </si>
   <si>
     <t>recht</t>
+  </si>
+  <si>
+    <t>ProcIdent</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2128,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,7 +2150,7 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" t="str">
         <f>D1</f>
@@ -2214,69 +2214,69 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E2" t="str">
         <f>D2</f>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:R2" si="1">E2</f>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="P2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" si="1"/>
-        <v>ProcID</v>
+        <v>ProcIdent</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>